<commit_message>
feat: remoção de arquivos desnecessários e adição de nova imagem GDre
</commit_message>
<xml_diff>
--- a/vigas.xlsx
+++ b/vigas.xlsx
@@ -87,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +116,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -134,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -286,6 +292,13 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -331,8 +344,8 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -707,7 +720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -736,7 +749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -765,7 +778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -794,7 +807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -823,7 +836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -852,7 +865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -881,7 +894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -910,7 +923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
@@ -939,7 +952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -968,7 +981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -997,7 +1010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1026,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
@@ -1055,7 +1068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1084,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -1113,7 +1126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="10" t="s">
         <v>21</v>
       </c>

</xml_diff>